<commit_message>
add: Document Kelengkapan Sidang dan HKI
</commit_message>
<xml_diff>
--- a/docs/bimbingan/report-bimbingan.xlsx
+++ b/docs/bimbingan/report-bimbingan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faisalamir/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faisalamir/StudioProjects/nutrition-framework/docs/bimbingan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CD198D7-265A-D84D-9749-F2259EBCC88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA8F322-B164-8B4F-BE00-A1217F2E3DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{6439F74A-64D4-7D41-AEB4-E672841D3A57}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6439F74A-64D4-7D41-AEB4-E672841D3A57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Log Bimbingan</t>
   </si>
@@ -47,6 +47,30 @@
   </si>
   <si>
     <t>Catatan</t>
+  </si>
+  <si>
+    <t>Bimbingan Seputar Judul</t>
+  </si>
+  <si>
+    <t>Bimbingan Bab 1</t>
+  </si>
+  <si>
+    <t>Bimbingan Rumusan Masalah</t>
+  </si>
+  <si>
+    <t>Bimbingan Metodologi Masalah</t>
+  </si>
+  <si>
+    <t>Bimbingan Tinjauan Pustaka</t>
+  </si>
+  <si>
+    <t>Bimbingan Pengerjaan Project</t>
+  </si>
+  <si>
+    <t>Bimbingan Pengajuan HKI</t>
+  </si>
+  <si>
+    <t>Bimbingan Seputar Pengganti Sidang</t>
   </si>
 </sst>
 </file>
@@ -400,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB11CB68-71C2-EE40-AC35-D0C65BB88A52}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,6 +464,9 @@
       <c r="D5" s="2">
         <v>0.625</v>
       </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6">
@@ -451,6 +478,9 @@
       <c r="D6" s="2">
         <v>0.66666666666666696</v>
       </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7">
@@ -460,7 +490,10 @@
         <v>44371</v>
       </c>
       <c r="D7" s="2">
-        <v>0.70833333333333304</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -471,7 +504,10 @@
         <v>44373</v>
       </c>
       <c r="D8" s="2">
-        <v>0.75</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -482,7 +518,10 @@
         <v>44375</v>
       </c>
       <c r="D9" s="2">
-        <v>0.79166666666666696</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -493,7 +532,10 @@
         <v>44501</v>
       </c>
       <c r="D10" s="2">
-        <v>0.83333333333333304</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -504,7 +546,10 @@
         <v>44511</v>
       </c>
       <c r="D11" s="2">
-        <v>0.875</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -515,7 +560,10 @@
         <v>44517</v>
       </c>
       <c r="D12" s="2">
-        <v>0.91666666666666696</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -526,7 +574,10 @@
         <v>44532</v>
       </c>
       <c r="D13" s="2">
-        <v>0.95833333333333304</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -537,7 +588,10 @@
         <v>44554</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -548,7 +602,52 @@
         <v>44543</v>
       </c>
       <c r="D15" s="2">
-        <v>1.0416666666666701</v>
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44566</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44567</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44576</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>